<commit_message>
Recognised related studies which includes survey
</commit_message>
<xml_diff>
--- a/Citations.xlsx
+++ b/Citations.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songhokun/Documents/Current studies/2DV50E/2019VT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4994E9-341B-F94F-B172-C92DD1868448}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0EAB99-6B47-D344-A059-B071F5E789CD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9680" yWindow="460" windowWidth="19100" windowHeight="17540" xr2:uid="{4E9165AD-0711-45BF-9FB6-BA0D375FFC6D}"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="37420" windowHeight="23540" xr2:uid="{4E9165AD-0711-45BF-9FB6-BA0D375FFC6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary sort" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Not-included" sheetId="2" r:id="rId2"/>
+    <sheet name="Architecture" sheetId="3" r:id="rId3"/>
+    <sheet name="Channel" sheetId="5" r:id="rId4"/>
+    <sheet name="Attack" sheetId="4" r:id="rId5"/>
+    <sheet name="Content" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Primary sort'!$A$1:$I$41</definedName>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="164">
   <si>
     <t>DNS query name minimisation to improve privacy</t>
   </si>
@@ -966,13 +969,306 @@
   </si>
   <si>
     <t>Content, Channel</t>
+  </si>
+  <si>
+    <r>
+      <t>M Ambrosin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A Compagno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M Conti</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M Ambrosin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A Compagno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M Conti</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C Ghali</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>…</t>
+    </r>
+  </si>
+  <si>
+    <t>rfc8484</t>
+  </si>
+  <si>
+    <r>
+      <t>A Mohaisen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Z Gu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>K Ren</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Z Li</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L Njilla</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>B Imana</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A Korolova</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J Heidemann</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M Müller</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R van Rijswijk-Deij</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1024,8 +1320,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1050,6 +1368,17 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1060,11 +1389,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1109,8 +1439,21 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1424,10 +1767,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043A32CE-2111-4D2C-BBEC-22A97A9D8998}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1468,7 +1812,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1497,7 +1841,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1555,7 +1899,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1581,7 +1925,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1610,7 +1954,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -1639,7 +1983,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1668,7 +2012,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1695,7 +2039,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1721,7 +2065,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1747,7 +2091,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>30</v>
       </c>
@@ -1775,7 +2119,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -1801,7 +2145,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>36</v>
       </c>
@@ -1828,7 +2172,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>38</v>
       </c>
@@ -1881,7 +2225,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>43</v>
       </c>
@@ -1907,7 +2251,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>46</v>
       </c>
@@ -1936,7 +2280,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -1992,7 +2336,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
@@ -2018,7 +2362,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>58</v>
       </c>
@@ -2096,7 +2440,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>66</v>
       </c>
@@ -2125,7 +2469,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>68</v>
       </c>
@@ -2157,7 +2501,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>71</v>
       </c>
@@ -2177,7 +2521,7 @@
       </c>
       <c r="J27" s="11"/>
     </row>
-    <row r="28" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>74</v>
       </c>
@@ -2201,7 +2545,7 @@
       </c>
       <c r="J28" s="11"/>
     </row>
-    <row r="29" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>76</v>
       </c>
@@ -2225,7 +2569,7 @@
       </c>
       <c r="J29" s="11"/>
     </row>
-    <row r="30" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>79</v>
       </c>
@@ -2274,7 +2618,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>86</v>
       </c>
@@ -2328,8 +2672,8 @@
       </c>
       <c r="J33" s="19"/>
     </row>
-    <row r="34" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
+    <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="31" t="s">
         <v>90</v>
       </c>
       <c r="B34" s="23" t="s">
@@ -2352,7 +2696,7 @@
       </c>
       <c r="J34" s="19"/>
     </row>
-    <row r="35" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>93</v>
       </c>
@@ -2378,7 +2722,7 @@
       </c>
       <c r="J35" s="19"/>
     </row>
-    <row r="36" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>96</v>
       </c>
@@ -2402,7 +2746,7 @@
       </c>
       <c r="J36" s="19"/>
     </row>
-    <row r="37" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>98</v>
       </c>
@@ -2424,7 +2768,7 @@
       </c>
       <c r="J37" s="19"/>
     </row>
-    <row r="38" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>100</v>
       </c>
@@ -2448,8 +2792,8 @@
       </c>
       <c r="J38" s="19"/>
     </row>
-    <row r="39" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="25" t="s">
+    <row r="39" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="31" t="s">
         <v>103</v>
       </c>
       <c r="B39" s="23" t="s">
@@ -2541,7 +2885,13 @@
       <c r="J43" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I41" xr:uid="{3B266C66-141F-464D-B17E-FCDE6A75B69E}"/>
+  <autoFilter ref="A1:I41" xr:uid="{3B266C66-141F-464D-B17E-FCDE6A75B69E}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Overview"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="http://www.rfc-editor.org/info/rfc7816" xr:uid="{F96C40B5-EC9C-48C1-A5D2-B55E6009F3FE}"/>
     <hyperlink ref="B2" r:id="rId2" display="https://scholar.google.se/citations?user=PlJjdcwAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{A487C5FA-2136-42D3-95C2-DFEC39633669}"/>
@@ -2601,24 +2951,1279 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E382F3-B0D9-4F98-88D0-4EE20A65E94C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="81.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <v>2018</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>2018</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4">
+        <v>2018</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5">
+        <v>2018</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7">
+        <v>2015</v>
+      </c>
+      <c r="E7" t="s">
+        <v>150</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" t="s">
+        <v>151</v>
+      </c>
+      <c r="I7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8">
+        <v>2015</v>
+      </c>
+      <c r="E8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" t="s">
+        <v>152</v>
+      </c>
+      <c r="I8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9">
+        <v>2018</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" t="s">
+        <v>120</v>
+      </c>
+      <c r="I9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10">
+        <v>2017</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F10" t="s">
+        <v>133</v>
+      </c>
+      <c r="I10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11">
+        <v>2018</v>
+      </c>
+      <c r="E11" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12">
+        <v>2017</v>
+      </c>
+      <c r="E12" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.sciencedirect.com/science/article/pii/S2352864817300731" xr:uid="{9002B147-5340-384E-9A34-9C2612FF6B8D}"/>
+    <hyperlink ref="B2" r:id="rId2" display="https://scholar.google.se/citations?user=H20D2WIAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{10A5C411-9B50-5949-8DAB-D19F75FF80CB}"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://www.sciencedirect.com/science/article/pii/S0167404818300403" xr:uid="{DFDB8019-9D7B-2749-B640-55B8908497DA}"/>
+    <hyperlink ref="A4" r:id="rId4" display="https://dl.acm.org/citation.cfm?id=3278544" xr:uid="{26C075E8-6941-0944-8EE5-56CAAB33E115}"/>
+    <hyperlink ref="B4" r:id="rId5" display="https://scholar.google.se/citations?user=bN_de_QAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{4EB00633-4148-D248-98C8-A11E07D7ED8B}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://ant.isi.edu/events/dinr2016/P/p11.pdf" xr:uid="{6E99BB2E-9951-054B-9542-87F82876A33A}"/>
+    <hyperlink ref="A7" r:id="rId7" display="http://datatracker.ietf.org/meeting/92/agenda/dprive-drafts.pdf" xr:uid="{D3532AEA-CBE9-8C4B-AC45-C1B871E19807}"/>
+    <hyperlink ref="A8" r:id="rId8" display="https://datatracker.ietf.org/meeting/94/agenda/hrpc-drafts.pdf" xr:uid="{2C059C4C-9E1A-B646-B6FA-FDAFDFEDEE16}"/>
+    <hyperlink ref="A9" r:id="rId9" display="https://dl.acm.org/citation.cfm?id=3182660" xr:uid="{02B5AFFD-5B69-8C4C-90EB-64F80D167EEF}"/>
+    <hyperlink ref="A10" r:id="rId10" display="http://kops.uni-konstanz.de/handle/123456789/39940" xr:uid="{680E31D4-D35E-754A-A0E2-47120B573DA9}"/>
+    <hyperlink ref="A11" r:id="rId11" display="https://link.springer.com/chapter/10.1007/978-3-658-23727-1_13" xr:uid="{6F38E0F9-88A7-B048-A578-3AA9F391F25D}"/>
+    <hyperlink ref="B11" r:id="rId12" display="https://scholar.google.se/citations?user=XV4F9qMAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{F36BC041-6DB6-6345-8BAE-1D9860A56653}"/>
+    <hyperlink ref="A12" r:id="rId13" display="http://www.infocomm-journal.com/cjnis/CN/10.11959/j.issn.2096-109x.2017.00154" xr:uid="{B57C5B63-2816-8F49-9132-ADE93FB49D63}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A9E353E-44A0-4983-BF56-013E9CE0D947}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="71" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="24">
+        <v>2018</v>
+      </c>
+      <c r="D2" s="24">
+        <v>3</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="24">
+        <v>2016</v>
+      </c>
+      <c r="D3" s="24">
+        <v>1</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="24">
+        <v>2017</v>
+      </c>
+      <c r="D4" s="24">
+        <v>1</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://ieeexplore.ieee.org/abstract/document/8269274/" xr:uid="{AD75C69B-90BB-5345-9E33-0B63408BEB42}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://arxiv.org/abs/1610.00355" xr:uid="{78CAE2EA-AC06-B746-B710-2F1068DB2819}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://hal.inria.fr/tel-01654244/" xr:uid="{85959053-9BE4-244C-86DA-370F1C81213D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CE97E7-3282-0449-B491-0DD2C0AF72F8}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="73.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D2" s="1">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2014</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="19">
+        <v>2018</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="19">
+        <v>2014</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="http://www.rfc-editor.org/info/rfc7858" xr:uid="{AB026C3A-965C-A248-BFAA-BD17CE2BCA45}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://www.rfc-editor.org/rfc/pdfrfc/rfc8484.txt.pdf" xr:uid="{36215557-2CE3-D048-BC6D-5E1B20BDF33B}"/>
+    <hyperlink ref="A4" r:id="rId3" display="http://www.rfc-editor.org/info/rfc8094" xr:uid="{361B8C0F-F95F-1A4B-AAF7-0269A984E996}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://ieeexplore.ieee.org/abstract/document/7165976/" xr:uid="{28C31547-926D-074A-A0AD-7B6438A3F480}"/>
+    <hyperlink ref="A6" r:id="rId5" display="http://www.rfc-editor.org/info/rfc8310" xr:uid="{EAC80F84-0112-A440-8975-DAFD7B2D52F0}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://www.researchgate.net/profile/Hakiza_Bucuti/publication/269633026_Encrypted_DNS_An_opportunistic_encryption_protocol_extension_for_the_Domain_Name_System/links/54dc80230cf23fe133b1a42b/Encrypted-DNS-An-opportunistic-encryption-protocol-extension-for-the-Domain-Name-System.pdf" xr:uid="{62CF1210-630A-6C48-8D41-54DDE925704A}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://ieeexplore.ieee.org/abstract/document/8281726/" xr:uid="{F2A656C5-280B-5A43-BDDE-5A6B7AFF110A}"/>
+    <hyperlink ref="B8" r:id="rId8" display="https://scholar.google.se/citations?user=MS8zaE8AAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{21A9641C-33D7-4644-9B04-52EB0AF17C6B}"/>
+    <hyperlink ref="A9" r:id="rId9" display="http://open.nlnetlabs.nl/downloads/publications/privacy-analysis-of-dns-vanheugten.pdf" xr:uid="{847D8B68-0190-B84D-8CEF-CE3B972D3C73}"/>
+    <hyperlink ref="A10" r:id="rId10" display="https://www.sidnlabs.nl/paper.pdf" xr:uid="{BE6F0081-D8F6-A845-A20B-70A51081B011}"/>
+    <hyperlink ref="A11" r:id="rId11" display="https://www.net.in.tum.de/fileadmin/TUM/NET/NET-2014-08-1/NET-2014-08-1_18.pdf" xr:uid="{09860D2C-DB55-FD4F-9E51-10ECC4DA02F5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6007CA-EB5A-3D47-820C-CD0CB3FB8D9B}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="129.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D2" s="1">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>140</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="http://www.rfc-editor.org/info/rfc7624" xr:uid="{E6A98821-1909-6043-9C86-17F7151BFCA7}"/>
+    <hyperlink ref="B2" r:id="rId2" display="https://scholar.google.se/citations?user=TQJvJ1kAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{4CBEAF6C-EE8F-1545-BE25-6D755DC55D5D}"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://dl.acm.org/citation.cfm?id=2996770" xr:uid="{D049CBD3-4F69-0E47-845A-1F30A62FFA57}"/>
+    <hyperlink ref="A4" r:id="rId4" display="https://ieeexplore.ieee.org/abstract/document/7972981/" xr:uid="{771A2404-D5A6-094F-A0FD-4A46732406D5}"/>
+    <hyperlink ref="A5" r:id="rId5" display="https://gnunet.org/sites/default/files/mcb-en.pdf" xr:uid="{B21DAF5A-3C9D-3745-A853-FFB7622798B9}"/>
+    <hyperlink ref="B5" r:id="rId6" display="https://scholar.google.se/citations?user=SZI-MdYAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{43B21B6F-7CB5-1C44-B986-7B4CDA93BE32}"/>
+    <hyperlink ref="A6" r:id="rId7" display="https://www.cs.ucf.edu/~mohaisen/doc/djeff18.pdf" xr:uid="{B806B414-1943-8043-9065-A33C5CA779CC}"/>
+    <hyperlink ref="B6" r:id="rId8" display="https://scholar.google.se/citations?user=Dm52d9kAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{02902970-C143-E24A-B59D-744B10489692}"/>
+    <hyperlink ref="A7" r:id="rId9" display="https://link.springer.com/chapter/10.1007/978-3-658-21384-8_8" xr:uid="{DCDFDA2B-E823-BF43-BCAD-E2B15F35BCB9}"/>
+    <hyperlink ref="B7" r:id="rId10" display="https://scholar.google.se/citations?user=9T2H9aQAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{1E613BD6-6566-1B49-BD68-54EFEB8634B5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F69704F-8F9F-4C48-BA5B-AD5DE6DC751D}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="91.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>2016</v>
+      </c>
+      <c r="D2">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>2016</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4">
+        <v>2018</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5">
+        <v>2019</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6">
+        <v>2018</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7">
+        <v>2018</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8">
+        <v>2019</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" t="s">
+        <v>138</v>
+      </c>
+      <c r="H8" t="s">
+        <v>120</v>
+      </c>
+      <c r="I8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9" t="s">
+        <v>156</v>
+      </c>
+      <c r="I9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10">
+        <v>2018</v>
+      </c>
+      <c r="E10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" t="s">
+        <v>130</v>
+      </c>
+      <c r="I10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11">
+        <v>2014</v>
+      </c>
+      <c r="E11" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" t="s">
+        <v>138</v>
+      </c>
+      <c r="I11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="http://www.rfc-editor.org/info/rfc7816" xr:uid="{2858BC83-E289-0643-8703-F7AA731D9930}"/>
+    <hyperlink ref="B2" r:id="rId2" display="https://scholar.google.se/citations?user=PlJjdcwAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{17CEAF26-8B37-FB45-803A-78F27F2F60A3}"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://link.springer.com/chapter/10.1007/978-3-319-40667-1_17" xr:uid="{5F387967-C09C-7A4D-9F22-5C5AEF495DA4}"/>
+    <hyperlink ref="B3" r:id="rId4" display="https://scholar.google.se/citations?user=WLiTyjsAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{73B3A0A1-431A-1643-BCE3-CD3311E88ACB}"/>
+    <hyperlink ref="A4" r:id="rId5" display="https://ieeexplore.ieee.org/abstract/document/8316923/" xr:uid="{34497BDA-F9A1-E444-BEBB-E036AAFA6BF6}"/>
+    <hyperlink ref="A5" r:id="rId6" xr:uid="{6FB7F0C7-985B-8C44-B6A0-E98AA60959F5}"/>
+    <hyperlink ref="A6" r:id="rId7" display="https://ieeexplore.ieee.org/abstract/document/8514164/" xr:uid="{6649819B-848F-F949-991A-5EAD06215078}"/>
+    <hyperlink ref="A7" r:id="rId8" display="https://ant.isi.edu/~imana/presentations/Imana18b.pdf" xr:uid="{153B5383-AA0B-9A4B-987B-9C2D7FA21F43}"/>
+    <hyperlink ref="A8" r:id="rId9" display="https://onlinelibrary.wiley.com/doi/abs/10.1002/poi3.195" xr:uid="{A50120E6-CACD-3845-A4F2-6EA1A16CF8B2}"/>
+    <hyperlink ref="B8" r:id="rId10" display="https://scholar.google.se/citations?user=PROAnvEAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{F12A7264-FD97-5445-A822-7D66ED39DF8B}"/>
+    <hyperlink ref="A9" r:id="rId11" display="https://www.sidnlabs.nl/paper.pdf" xr:uid="{DB23777C-EF16-D848-8D19-BA043F663A28}"/>
+    <hyperlink ref="A10" r:id="rId12" display="https://ieeexplore.ieee.org/abstract/document/8456024/" xr:uid="{1A7F34F6-815A-824F-80A0-EC447243DE88}"/>
+    <hyperlink ref="A11" r:id="rId13" display="https://www.net.in.tum.de/fileadmin/TUM/NET/NET-2014-08-1/NET-2014-08-1_18.pdf" xr:uid="{1BA75084-270A-8C44-B010-6368B6C2F8B9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Experiment Design (Implementation chapter)
</commit_message>
<xml_diff>
--- a/Citations.xlsx
+++ b/Citations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songhokun/Documents/Current studies/2DV50E/2019VT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0EAB99-6B47-D344-A059-B071F5E789CD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE42C22-0167-6249-8264-48EE5ED776EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="37420" windowHeight="23540" xr2:uid="{4E9165AD-0711-45BF-9FB6-BA0D375FFC6D}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="50280" windowHeight="28340" xr2:uid="{4E9165AD-0711-45BF-9FB6-BA0D375FFC6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary sort" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="165">
   <si>
     <t>DNS query name minimisation to improve privacy</t>
   </si>
@@ -1262,6 +1262,9 @@
       </rPr>
       <t> </t>
     </r>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -1770,8 +1773,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" zoomScale="182" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1779,6 +1782,7 @@
     <col min="1" max="1" width="74.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" style="1" customWidth="1"/>
     <col min="3" max="4" width="9.1640625" style="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" style="1"/>
     <col min="8" max="10" width="9.1640625" style="1"/>
   </cols>
@@ -1925,7 +1929,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -2440,7 +2444,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>66</v>
       </c>
@@ -2521,7 +2525,7 @@
       </c>
       <c r="J27" s="11"/>
     </row>
-    <row r="28" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>74</v>
       </c>
@@ -2545,7 +2549,7 @@
       </c>
       <c r="J28" s="11"/>
     </row>
-    <row r="29" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>76</v>
       </c>
@@ -2618,7 +2622,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>86</v>
       </c>
@@ -2696,7 +2700,7 @@
       </c>
       <c r="J34" s="19"/>
     </row>
-    <row r="35" spans="1:10" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>93</v>
       </c>
@@ -2768,7 +2772,7 @@
       </c>
       <c r="J37" s="19"/>
     </row>
-    <row r="38" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>100</v>
       </c>
@@ -2888,6 +2892,7 @@
   <autoFilter ref="A1:I41" xr:uid="{3B266C66-141F-464D-B17E-FCDE6A75B69E}">
     <filterColumn colId="5">
       <filters>
+        <filter val="In-depth study"/>
         <filter val="Overview"/>
       </filters>
     </filterColumn>
@@ -3251,132 +3256,136 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A9E353E-44A0-4983-BF56-013E9CE0D947}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="71" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="C1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="E1" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="G1" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="H1" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="C2" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="24">
+      <c r="D2" s="24">
         <v>2018</v>
       </c>
-      <c r="D2" s="24">
+      <c r="E2" s="24">
         <v>3</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="F2" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="G2" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="I2" s="28" t="s">
+      <c r="H2" s="24"/>
+      <c r="I2" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="C3" s="24">
+      <c r="D3" s="24">
         <v>2016</v>
       </c>
-      <c r="D3" s="24">
+      <c r="E3" s="24">
         <v>1</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="F3" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="G3" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="I3" s="28" t="s">
+      <c r="H3" s="24"/>
+      <c r="I3" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" s="28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B4" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="C4" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="24">
+      <c r="D4" s="24">
         <v>2017</v>
       </c>
-      <c r="D4" s="24">
+      <c r="E4" s="24">
         <v>1</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="F4" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="G4" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="I4" s="28" t="s">
+      <c r="H4" s="24"/>
+      <c r="I4" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="28" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://ieeexplore.ieee.org/abstract/document/8269274/" xr:uid="{AD75C69B-90BB-5345-9E33-0B63408BEB42}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://arxiv.org/abs/1610.00355" xr:uid="{78CAE2EA-AC06-B746-B710-2F1068DB2819}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://hal.inria.fr/tel-01654244/" xr:uid="{85959053-9BE4-244C-86DA-370F1C81213D}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://ieeexplore.ieee.org/abstract/document/8269274/" xr:uid="{AD75C69B-90BB-5345-9E33-0B63408BEB42}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://arxiv.org/abs/1610.00355" xr:uid="{78CAE2EA-AC06-B746-B710-2F1068DB2819}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://hal.inria.fr/tel-01654244/" xr:uid="{85959053-9BE4-244C-86DA-370F1C81213D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3384,320 +3393,324 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CE97E7-3282-0449-B491-0DD2C0AF72F8}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J11" sqref="A1:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="73.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>2016</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>2018</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>2017</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>122</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>2015</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>122</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>2018</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>122</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>2014</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>122</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>2017</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>122</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B9" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="C9" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="19">
+      <c r="D9" s="19">
         <v>2018</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="19"/>
+      <c r="F9" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="G9" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="21" t="s">
+      <c r="H9" s="20"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="21" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="C10" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="19"/>
       <c r="D10" s="19"/>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="19"/>
+      <c r="F10" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="G10" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="21" t="s">
+      <c r="H10" s="20"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="21" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="C11" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="19">
+      <c r="D11" s="19">
         <v>2014</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="19"/>
+      <c r="F11" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="G11" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="21" t="s">
+      <c r="H11" s="20"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="21" t="s">
         <v>105</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://www.rfc-editor.org/info/rfc7858" xr:uid="{AB026C3A-965C-A248-BFAA-BD17CE2BCA45}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://www.rfc-editor.org/rfc/pdfrfc/rfc8484.txt.pdf" xr:uid="{36215557-2CE3-D048-BC6D-5E1B20BDF33B}"/>
-    <hyperlink ref="A4" r:id="rId3" display="http://www.rfc-editor.org/info/rfc8094" xr:uid="{361B8C0F-F95F-1A4B-AAF7-0269A984E996}"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://ieeexplore.ieee.org/abstract/document/7165976/" xr:uid="{28C31547-926D-074A-A0AD-7B6438A3F480}"/>
-    <hyperlink ref="A6" r:id="rId5" display="http://www.rfc-editor.org/info/rfc8310" xr:uid="{EAC80F84-0112-A440-8975-DAFD7B2D52F0}"/>
-    <hyperlink ref="A7" r:id="rId6" display="https://www.researchgate.net/profile/Hakiza_Bucuti/publication/269633026_Encrypted_DNS_An_opportunistic_encryption_protocol_extension_for_the_Domain_Name_System/links/54dc80230cf23fe133b1a42b/Encrypted-DNS-An-opportunistic-encryption-protocol-extension-for-the-Domain-Name-System.pdf" xr:uid="{62CF1210-630A-6C48-8D41-54DDE925704A}"/>
-    <hyperlink ref="A8" r:id="rId7" display="https://ieeexplore.ieee.org/abstract/document/8281726/" xr:uid="{F2A656C5-280B-5A43-BDDE-5A6B7AFF110A}"/>
-    <hyperlink ref="B8" r:id="rId8" display="https://scholar.google.se/citations?user=MS8zaE8AAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{21A9641C-33D7-4644-9B04-52EB0AF17C6B}"/>
-    <hyperlink ref="A9" r:id="rId9" display="http://open.nlnetlabs.nl/downloads/publications/privacy-analysis-of-dns-vanheugten.pdf" xr:uid="{847D8B68-0190-B84D-8CEF-CE3B972D3C73}"/>
-    <hyperlink ref="A10" r:id="rId10" display="https://www.sidnlabs.nl/paper.pdf" xr:uid="{BE6F0081-D8F6-A845-A20B-70A51081B011}"/>
-    <hyperlink ref="A11" r:id="rId11" display="https://www.net.in.tum.de/fileadmin/TUM/NET/NET-2014-08-1/NET-2014-08-1_18.pdf" xr:uid="{09860D2C-DB55-FD4F-9E51-10ECC4DA02F5}"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://www.rfc-editor.org/info/rfc7858" xr:uid="{AB026C3A-965C-A248-BFAA-BD17CE2BCA45}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://www.rfc-editor.org/rfc/pdfrfc/rfc8484.txt.pdf" xr:uid="{36215557-2CE3-D048-BC6D-5E1B20BDF33B}"/>
+    <hyperlink ref="B4" r:id="rId3" display="http://www.rfc-editor.org/info/rfc8094" xr:uid="{361B8C0F-F95F-1A4B-AAF7-0269A984E996}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://ieeexplore.ieee.org/abstract/document/7165976/" xr:uid="{28C31547-926D-074A-A0AD-7B6438A3F480}"/>
+    <hyperlink ref="B6" r:id="rId5" display="http://www.rfc-editor.org/info/rfc8310" xr:uid="{EAC80F84-0112-A440-8975-DAFD7B2D52F0}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://www.researchgate.net/profile/Hakiza_Bucuti/publication/269633026_Encrypted_DNS_An_opportunistic_encryption_protocol_extension_for_the_Domain_Name_System/links/54dc80230cf23fe133b1a42b/Encrypted-DNS-An-opportunistic-encryption-protocol-extension-for-the-Domain-Name-System.pdf" xr:uid="{62CF1210-630A-6C48-8D41-54DDE925704A}"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://ieeexplore.ieee.org/abstract/document/8281726/" xr:uid="{F2A656C5-280B-5A43-BDDE-5A6B7AFF110A}"/>
+    <hyperlink ref="C8" r:id="rId8" display="https://scholar.google.se/citations?user=MS8zaE8AAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{21A9641C-33D7-4644-9B04-52EB0AF17C6B}"/>
+    <hyperlink ref="B9" r:id="rId9" display="http://open.nlnetlabs.nl/downloads/publications/privacy-analysis-of-dns-vanheugten.pdf" xr:uid="{847D8B68-0190-B84D-8CEF-CE3B972D3C73}"/>
+    <hyperlink ref="B10" r:id="rId10" display="https://www.sidnlabs.nl/paper.pdf" xr:uid="{BE6F0081-D8F6-A845-A20B-70A51081B011}"/>
+    <hyperlink ref="B11" r:id="rId11" display="https://www.net.in.tum.de/fileadmin/TUM/NET/NET-2014-08-1/NET-2014-08-1_18.pdf" xr:uid="{09860D2C-DB55-FD4F-9E51-10ECC4DA02F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3705,217 +3718,225 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6007CA-EB5A-3D47-820C-CD0CB3FB8D9B}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="129.1640625" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.83203125" customWidth="1"/>
+    <col min="3" max="3" width="81" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1">
+      <c r="E2" s="1">
         <v>2015</v>
       </c>
-      <c r="D2" s="1">
+      <c r="F2" s="1">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="1">
+      <c r="E3" s="1">
         <v>2016</v>
       </c>
-      <c r="D3" s="1">
+      <c r="F3" s="1">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>140</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C4" s="1">
+      <c r="E4" s="1">
         <v>2017</v>
       </c>
-      <c r="D4" s="1">
+      <c r="F4" s="1">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>140</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="C5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="1">
+      <c r="E5" s="1">
         <v>2017</v>
       </c>
-      <c r="D5" s="1">
+      <c r="F5" s="1">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>140</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>136</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="C6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="1">
+      <c r="E6" s="1">
         <v>2018</v>
       </c>
-      <c r="D6" s="1">
+      <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>140</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="1">
+      <c r="E7" s="1">
         <v>2018</v>
       </c>
-      <c r="D7" s="1">
+      <c r="F7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>140</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://www.rfc-editor.org/info/rfc7624" xr:uid="{E6A98821-1909-6043-9C86-17F7151BFCA7}"/>
-    <hyperlink ref="B2" r:id="rId2" display="https://scholar.google.se/citations?user=TQJvJ1kAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{4CBEAF6C-EE8F-1545-BE25-6D755DC55D5D}"/>
-    <hyperlink ref="A3" r:id="rId3" display="https://dl.acm.org/citation.cfm?id=2996770" xr:uid="{D049CBD3-4F69-0E47-845A-1F30A62FFA57}"/>
-    <hyperlink ref="A4" r:id="rId4" display="https://ieeexplore.ieee.org/abstract/document/7972981/" xr:uid="{771A2404-D5A6-094F-A0FD-4A46732406D5}"/>
-    <hyperlink ref="A5" r:id="rId5" display="https://gnunet.org/sites/default/files/mcb-en.pdf" xr:uid="{B21DAF5A-3C9D-3745-A853-FFB7622798B9}"/>
-    <hyperlink ref="B5" r:id="rId6" display="https://scholar.google.se/citations?user=SZI-MdYAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{43B21B6F-7CB5-1C44-B986-7B4CDA93BE32}"/>
-    <hyperlink ref="A6" r:id="rId7" display="https://www.cs.ucf.edu/~mohaisen/doc/djeff18.pdf" xr:uid="{B806B414-1943-8043-9065-A33C5CA779CC}"/>
-    <hyperlink ref="B6" r:id="rId8" display="https://scholar.google.se/citations?user=Dm52d9kAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{02902970-C143-E24A-B59D-744B10489692}"/>
-    <hyperlink ref="A7" r:id="rId9" display="https://link.springer.com/chapter/10.1007/978-3-658-21384-8_8" xr:uid="{DCDFDA2B-E823-BF43-BCAD-E2B15F35BCB9}"/>
-    <hyperlink ref="B7" r:id="rId10" display="https://scholar.google.se/citations?user=9T2H9aQAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{1E613BD6-6566-1B49-BD68-54EFEB8634B5}"/>
+    <hyperlink ref="C2" r:id="rId1" display="http://www.rfc-editor.org/info/rfc7624" xr:uid="{E6A98821-1909-6043-9C86-17F7151BFCA7}"/>
+    <hyperlink ref="D2" r:id="rId2" display="https://scholar.google.se/citations?user=TQJvJ1kAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{4CBEAF6C-EE8F-1545-BE25-6D755DC55D5D}"/>
+    <hyperlink ref="C3" r:id="rId3" display="https://dl.acm.org/citation.cfm?id=2996770" xr:uid="{D049CBD3-4F69-0E47-845A-1F30A62FFA57}"/>
+    <hyperlink ref="C4" r:id="rId4" display="https://ieeexplore.ieee.org/abstract/document/7972981/" xr:uid="{771A2404-D5A6-094F-A0FD-4A46732406D5}"/>
+    <hyperlink ref="C5" r:id="rId5" display="https://gnunet.org/sites/default/files/mcb-en.pdf" xr:uid="{B21DAF5A-3C9D-3745-A853-FFB7622798B9}"/>
+    <hyperlink ref="D5" r:id="rId6" display="https://scholar.google.se/citations?user=SZI-MdYAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{43B21B6F-7CB5-1C44-B986-7B4CDA93BE32}"/>
+    <hyperlink ref="C6" r:id="rId7" display="https://www.cs.ucf.edu/~mohaisen/doc/djeff18.pdf" xr:uid="{B806B414-1943-8043-9065-A33C5CA779CC}"/>
+    <hyperlink ref="D6" r:id="rId8" display="https://scholar.google.se/citations?user=Dm52d9kAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{02902970-C143-E24A-B59D-744B10489692}"/>
+    <hyperlink ref="C7" r:id="rId9" display="https://link.springer.com/chapter/10.1007/978-3-658-21384-8_8" xr:uid="{DCDFDA2B-E823-BF43-BCAD-E2B15F35BCB9}"/>
+    <hyperlink ref="D7" r:id="rId10" display="https://scholar.google.se/citations?user=9T2H9aQAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{1E613BD6-6566-1B49-BD68-54EFEB8634B5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3923,306 +3944,310 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F69704F-8F9F-4C48-BA5B-AD5DE6DC751D}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="91.33203125" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>121</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>126</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>127</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>128</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>119</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>2016</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>33</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>129</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>123</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>131</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>132</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2016</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>129</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>130</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>134</v>
       </c>
-      <c r="H3" t="s">
-        <v>120</v>
-      </c>
       <c r="I3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>66</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>161</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>2018</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>129</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>130</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>148</v>
       </c>
-      <c r="H4" t="s">
-        <v>120</v>
-      </c>
       <c r="I4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>68</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>69</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>2019</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>129</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>123</v>
       </c>
-      <c r="H5" t="s">
-        <v>120</v>
-      </c>
       <c r="I5" t="s">
+        <v>120</v>
+      </c>
+      <c r="J5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>79</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>80</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>2018</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>129</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>123</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>86</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>162</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>2018</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>129</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>130</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>137</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>87</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>88</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>2019</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>129</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>138</v>
       </c>
-      <c r="H8" t="s">
-        <v>120</v>
-      </c>
       <c r="I8" t="s">
+        <v>120</v>
+      </c>
+      <c r="J8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>98</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>163</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>157</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>156</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>100</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>101</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>2018</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>129</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>130</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>103</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>104</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>2014</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>157</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>138</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>105</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://www.rfc-editor.org/info/rfc7816" xr:uid="{2858BC83-E289-0643-8703-F7AA731D9930}"/>
-    <hyperlink ref="B2" r:id="rId2" display="https://scholar.google.se/citations?user=PlJjdcwAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{17CEAF26-8B37-FB45-803A-78F27F2F60A3}"/>
-    <hyperlink ref="A3" r:id="rId3" display="https://link.springer.com/chapter/10.1007/978-3-319-40667-1_17" xr:uid="{5F387967-C09C-7A4D-9F22-5C5AEF495DA4}"/>
-    <hyperlink ref="B3" r:id="rId4" display="https://scholar.google.se/citations?user=WLiTyjsAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{73B3A0A1-431A-1643-BCE3-CD3311E88ACB}"/>
-    <hyperlink ref="A4" r:id="rId5" display="https://ieeexplore.ieee.org/abstract/document/8316923/" xr:uid="{34497BDA-F9A1-E444-BEBB-E036AAFA6BF6}"/>
-    <hyperlink ref="A5" r:id="rId6" xr:uid="{6FB7F0C7-985B-8C44-B6A0-E98AA60959F5}"/>
-    <hyperlink ref="A6" r:id="rId7" display="https://ieeexplore.ieee.org/abstract/document/8514164/" xr:uid="{6649819B-848F-F949-991A-5EAD06215078}"/>
-    <hyperlink ref="A7" r:id="rId8" display="https://ant.isi.edu/~imana/presentations/Imana18b.pdf" xr:uid="{153B5383-AA0B-9A4B-987B-9C2D7FA21F43}"/>
-    <hyperlink ref="A8" r:id="rId9" display="https://onlinelibrary.wiley.com/doi/abs/10.1002/poi3.195" xr:uid="{A50120E6-CACD-3845-A4F2-6EA1A16CF8B2}"/>
-    <hyperlink ref="B8" r:id="rId10" display="https://scholar.google.se/citations?user=PROAnvEAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{F12A7264-FD97-5445-A822-7D66ED39DF8B}"/>
-    <hyperlink ref="A9" r:id="rId11" display="https://www.sidnlabs.nl/paper.pdf" xr:uid="{DB23777C-EF16-D848-8D19-BA043F663A28}"/>
-    <hyperlink ref="A10" r:id="rId12" display="https://ieeexplore.ieee.org/abstract/document/8456024/" xr:uid="{1A7F34F6-815A-824F-80A0-EC447243DE88}"/>
-    <hyperlink ref="A11" r:id="rId13" display="https://www.net.in.tum.de/fileadmin/TUM/NET/NET-2014-08-1/NET-2014-08-1_18.pdf" xr:uid="{1BA75084-270A-8C44-B010-6368B6C2F8B9}"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://www.rfc-editor.org/info/rfc7816" xr:uid="{2858BC83-E289-0643-8703-F7AA731D9930}"/>
+    <hyperlink ref="C2" r:id="rId2" display="https://scholar.google.se/citations?user=PlJjdcwAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{17CEAF26-8B37-FB45-803A-78F27F2F60A3}"/>
+    <hyperlink ref="B3" r:id="rId3" display="https://link.springer.com/chapter/10.1007/978-3-319-40667-1_17" xr:uid="{5F387967-C09C-7A4D-9F22-5C5AEF495DA4}"/>
+    <hyperlink ref="C3" r:id="rId4" display="https://scholar.google.se/citations?user=WLiTyjsAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{73B3A0A1-431A-1643-BCE3-CD3311E88ACB}"/>
+    <hyperlink ref="B4" r:id="rId5" display="https://ieeexplore.ieee.org/abstract/document/8316923/" xr:uid="{34497BDA-F9A1-E444-BEBB-E036AAFA6BF6}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{6FB7F0C7-985B-8C44-B6A0-E98AA60959F5}"/>
+    <hyperlink ref="B6" r:id="rId7" display="https://ieeexplore.ieee.org/abstract/document/8514164/" xr:uid="{6649819B-848F-F949-991A-5EAD06215078}"/>
+    <hyperlink ref="B7" r:id="rId8" display="https://ant.isi.edu/~imana/presentations/Imana18b.pdf" xr:uid="{153B5383-AA0B-9A4B-987B-9C2D7FA21F43}"/>
+    <hyperlink ref="B8" r:id="rId9" display="https://onlinelibrary.wiley.com/doi/abs/10.1002/poi3.195" xr:uid="{A50120E6-CACD-3845-A4F2-6EA1A16CF8B2}"/>
+    <hyperlink ref="C8" r:id="rId10" display="https://scholar.google.se/citations?user=PROAnvEAAAAJ&amp;hl=sv&amp;oi=sra" xr:uid="{F12A7264-FD97-5445-A822-7D66ED39DF8B}"/>
+    <hyperlink ref="B9" r:id="rId11" display="https://www.sidnlabs.nl/paper.pdf" xr:uid="{DB23777C-EF16-D848-8D19-BA043F663A28}"/>
+    <hyperlink ref="B10" r:id="rId12" display="https://ieeexplore.ieee.org/abstract/document/8456024/" xr:uid="{1A7F34F6-815A-824F-80A0-EC447243DE88}"/>
+    <hyperlink ref="B11" r:id="rId13" display="https://www.net.in.tum.de/fileadmin/TUM/NET/NET-2014-08-1/NET-2014-08-1_18.pdf" xr:uid="{1BA75084-270A-8C44-B010-6368B6C2F8B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>